<commit_message>
Add new Excel files for Musikkvideouka 2025 and Musikkvideouka 2
- Created MAL_Musikkvideouka2025.xlsx with 9446 rows of data.
- Created MAL_Musikkvideouka_2.xlsx with 9802 rows of data.
- Included necessary XML files and relationships for both Excel files.
</commit_message>
<xml_diff>
--- a/MAL_Musikkvideouka.xlsx
+++ b/MAL_Musikkvideouka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vestfoldfylke-my.sharepoint.com/personal/torgeir_bull_vestfoldfylke_no/Documents/Dokumenter/2025-2026/Annet/Musikkvideouka 2025/Musikkvideouka_V10_FIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{F36FA709-59AC-444C-A0C0-639CD79B3C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D92D3D4C-3972-1146-AB5F-7BE5BCA67E20}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{F36FA709-59AC-444C-A0C0-639CD79B3C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24B1B35B-68F2-AC46-A8F6-53038475A1C4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Navn</t>
   </si>
@@ -88,12 +88,6 @@
     <t>Gruppe 18</t>
   </si>
   <si>
-    <t>Gruppe 19</t>
-  </si>
-  <si>
-    <t>Gruppe 20</t>
-  </si>
-  <si>
     <t>/album_covers/artist_1.png</t>
   </si>
   <si>
@@ -143,19 +137,13 @@
   </si>
   <si>
     <t>/album_covers/artist_18.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_19.png</t>
-  </si>
-  <si>
-    <t>/album_covers/artist_20.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -180,15 +168,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,21 +207,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -566,247 +558,237 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="108.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C4" s="3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C9" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C14" s="3">
         <v>34</v>
       </c>
-      <c r="C13" s="1">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C16" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="18" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="1">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C18" s="3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C19" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2</v>
-      </c>
-    </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
+      <c r="A21" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C1 A3 A2 A18 A11 C11 A10 A6 C6 A5 A4 C4 C3 C5 A7 C7 A8 C8 A9 C9 C10 A12 C12 A13 C13 A14 C14 A15 C15 A16 C16 A17 C17 C18" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C1 A3 A2 A18 A11 C11 A10 A6 C6 A5 A4 C4 C3 C5 A7 C7 A8 C8 A9 C9 C10 A12 C12 A13 C13 A14 C14 A15 C15 A16 C16 A17 C17" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update MAL_Musikkvideouka.xlsx with new data
</commit_message>
<xml_diff>
--- a/MAL_Musikkvideouka.xlsx
+++ b/MAL_Musikkvideouka.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vestfoldfylke-my.sharepoint.com/personal/torgeir_bull_vestfoldfylke_no/Documents/Dokumenter/2025-2026/Annet/Musikkvideouka 2025/Musikkvideouka_V10_FIN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vestfoldfylke-my.sharepoint.com/personal/torgeir_bull_vestfoldfylke_no/Documents/Dokumenter/2025-2026/Annet/Musikkvideouka 2025/Musikkvideouka2025/Musikkvideouka-appv2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{F36FA709-59AC-444C-A0C0-639CD79B3C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F401855-1DDA-0F44-AB97-C0392010937C}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{F36FA709-59AC-444C-A0C0-639CD79B3C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07F7768C-B28F-496D-ABAE-C904C3FA6DA2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Navn</t>
   </si>
@@ -137,22 +137,32 @@
   </si>
   <si>
     <t>/album_covers/artist_18.png</t>
+  </si>
+  <si>
+    <t>Gruppe 19</t>
+  </si>
+  <si>
+    <t>Gruppe 20</t>
+  </si>
+  <si>
+    <t>Gruppe 21</t>
+  </si>
+  <si>
+    <t>/album_covers/artist_19.png</t>
+  </si>
+  <si>
+    <t>/album_covers/artist_20.png</t>
+  </si>
+  <si>
+    <t>/album_covers/artist_21.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -210,12 +220,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -231,10 +240,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,237 +564,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:C1 A3 A2 A18 A11 A10 A6 A5 A4 A7 A8 A9 A12 A13 A14 A15 A16 A17" numberStoredAsText="1"/>

</xml_diff>